<commit_message>
Changing R23 100 Ohm to 10k, small change, does not change functionallity.
</commit_message>
<xml_diff>
--- a/Component_Placement_Sheet.xlsx
+++ b/Component_Placement_Sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/saxani/My Drive/CosmicWatch/GitHub/CosmicWatch-Desktop-Muon-Detector-v3X/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABC41F7A-15E4-C34A-B80D-D726C240DA95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5D04C37-D36B-B04B-A87B-F5500CFD8A1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1100" yWindow="760" windowWidth="24540" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="209">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="212">
   <si>
     <t>1k</t>
   </si>
@@ -634,9 +634,6 @@
     <t>C3,C2,C19,C17,C20</t>
   </si>
   <si>
-    <t>R9,R29,R28,R8,R18,R23</t>
-  </si>
-  <si>
     <t>R10,R26,R14</t>
   </si>
   <si>
@@ -662,6 +659,18 @@
   </si>
   <si>
     <t>4x screws to mount the standoffs to SiPM board</t>
+  </si>
+  <si>
+    <t>R23</t>
+  </si>
+  <si>
+    <t>10k</t>
+  </si>
+  <si>
+    <t>RES SMD 10k OHM 1% 1/8W 0805</t>
+  </si>
+  <si>
+    <t>R9,R29,R28,R8,R18</t>
   </si>
 </sst>
 </file>
@@ -1121,13 +1130,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>417992</xdr:colOff>
-      <xdr:row>34</xdr:row>
+      <xdr:row>35</xdr:row>
       <xdr:rowOff>90650</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>786893</xdr:colOff>
-      <xdr:row>34</xdr:row>
+      <xdr:row>35</xdr:row>
       <xdr:rowOff>428413</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1165,13 +1174,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>286440</xdr:colOff>
-      <xdr:row>14</xdr:row>
+      <xdr:row>15</xdr:row>
       <xdr:rowOff>57321</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>912593</xdr:colOff>
-      <xdr:row>14</xdr:row>
+      <xdr:row>15</xdr:row>
       <xdr:rowOff>486505</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1209,13 +1218,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>438379</xdr:colOff>
-      <xdr:row>23</xdr:row>
+      <xdr:row>24</xdr:row>
       <xdr:rowOff>137405</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>722255</xdr:colOff>
-      <xdr:row>23</xdr:row>
+      <xdr:row>24</xdr:row>
       <xdr:rowOff>480305</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1253,13 +1262,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>356109</xdr:colOff>
-      <xdr:row>31</xdr:row>
+      <xdr:row>32</xdr:row>
       <xdr:rowOff>109052</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>868394</xdr:colOff>
-      <xdr:row>31</xdr:row>
+      <xdr:row>32</xdr:row>
       <xdr:rowOff>472667</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1297,13 +1306,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>343843</xdr:colOff>
-      <xdr:row>33</xdr:row>
+      <xdr:row>34</xdr:row>
       <xdr:rowOff>87039</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>774216</xdr:colOff>
-      <xdr:row>33</xdr:row>
+      <xdr:row>34</xdr:row>
       <xdr:rowOff>455339</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1341,13 +1350,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>374879</xdr:colOff>
-      <xdr:row>35</xdr:row>
+      <xdr:row>36</xdr:row>
       <xdr:rowOff>106802</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>743179</xdr:colOff>
-      <xdr:row>35</xdr:row>
+      <xdr:row>36</xdr:row>
       <xdr:rowOff>438087</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1385,13 +1394,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>425678</xdr:colOff>
-      <xdr:row>38</xdr:row>
+      <xdr:row>39</xdr:row>
       <xdr:rowOff>132202</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>751499</xdr:colOff>
-      <xdr:row>38</xdr:row>
+      <xdr:row>39</xdr:row>
       <xdr:rowOff>437002</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1429,13 +1438,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>374879</xdr:colOff>
-      <xdr:row>39</xdr:row>
+      <xdr:row>40</xdr:row>
       <xdr:rowOff>81402</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>694079</xdr:colOff>
-      <xdr:row>39</xdr:row>
+      <xdr:row>40</xdr:row>
       <xdr:rowOff>437002</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1473,13 +1482,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>412979</xdr:colOff>
-      <xdr:row>40</xdr:row>
+      <xdr:row>41</xdr:row>
       <xdr:rowOff>94102</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>783493</xdr:colOff>
-      <xdr:row>40</xdr:row>
+      <xdr:row>41</xdr:row>
       <xdr:rowOff>475102</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1517,13 +1526,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>400279</xdr:colOff>
-      <xdr:row>41</xdr:row>
+      <xdr:row>42</xdr:row>
       <xdr:rowOff>119502</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>752250</xdr:colOff>
-      <xdr:row>41</xdr:row>
+      <xdr:row>42</xdr:row>
       <xdr:rowOff>424302</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1561,13 +1570,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>435778</xdr:colOff>
-      <xdr:row>48</xdr:row>
+      <xdr:row>49</xdr:row>
       <xdr:rowOff>68702</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>765978</xdr:colOff>
-      <xdr:row>48</xdr:row>
+      <xdr:row>49</xdr:row>
       <xdr:rowOff>453416</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1605,7 +1614,7 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>257978</xdr:colOff>
-      <xdr:row>50</xdr:row>
+      <xdr:row>51</xdr:row>
       <xdr:rowOff>132202</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="533400" cy="278571"/>
@@ -1644,13 +1653,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>346878</xdr:colOff>
-      <xdr:row>51</xdr:row>
+      <xdr:row>52</xdr:row>
       <xdr:rowOff>106802</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>818366</xdr:colOff>
-      <xdr:row>51</xdr:row>
+      <xdr:row>52</xdr:row>
       <xdr:rowOff>386202</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1688,13 +1697,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>308779</xdr:colOff>
-      <xdr:row>61</xdr:row>
+      <xdr:row>62</xdr:row>
       <xdr:rowOff>119705</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>816779</xdr:colOff>
-      <xdr:row>61</xdr:row>
+      <xdr:row>62</xdr:row>
       <xdr:rowOff>457200</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1732,13 +1741,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>405176</xdr:colOff>
-      <xdr:row>63</xdr:row>
+      <xdr:row>64</xdr:row>
       <xdr:rowOff>96703</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>735376</xdr:colOff>
-      <xdr:row>63</xdr:row>
+      <xdr:row>64</xdr:row>
       <xdr:rowOff>512174</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1776,13 +1785,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>300090</xdr:colOff>
-      <xdr:row>62</xdr:row>
+      <xdr:row>63</xdr:row>
       <xdr:rowOff>123514</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>891910</xdr:colOff>
-      <xdr:row>62</xdr:row>
+      <xdr:row>63</xdr:row>
       <xdr:rowOff>452303</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1820,13 +1829,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>235178</xdr:colOff>
-      <xdr:row>59</xdr:row>
+      <xdr:row>60</xdr:row>
       <xdr:rowOff>129602</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>902211</xdr:colOff>
-      <xdr:row>59</xdr:row>
+      <xdr:row>60</xdr:row>
       <xdr:rowOff>472502</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1864,13 +1873,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>368417</xdr:colOff>
-      <xdr:row>58</xdr:row>
+      <xdr:row>59</xdr:row>
       <xdr:rowOff>39666</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>930349</xdr:colOff>
-      <xdr:row>58</xdr:row>
+      <xdr:row>59</xdr:row>
       <xdr:rowOff>522266</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1908,7 +1917,7 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>422113</xdr:colOff>
-      <xdr:row>36</xdr:row>
+      <xdr:row>37</xdr:row>
       <xdr:rowOff>84968</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="355600" cy="348468"/>
@@ -1947,13 +1956,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>367230</xdr:colOff>
-      <xdr:row>37</xdr:row>
+      <xdr:row>38</xdr:row>
       <xdr:rowOff>91807</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>856868</xdr:colOff>
-      <xdr:row>37</xdr:row>
+      <xdr:row>38</xdr:row>
       <xdr:rowOff>486293</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1991,13 +2000,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>346406</xdr:colOff>
-      <xdr:row>57</xdr:row>
+      <xdr:row>58</xdr:row>
       <xdr:rowOff>138170</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>872767</xdr:colOff>
-      <xdr:row>57</xdr:row>
+      <xdr:row>58</xdr:row>
       <xdr:rowOff>486376</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -3079,10 +3088,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:J68"/>
+  <dimension ref="A1:J69"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A51" zoomScale="75" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E57" sqref="E57"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="75" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.33203125" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -3257,7 +3266,7 @@
         <v>4</v>
       </c>
       <c r="B8" s="15" t="s">
-        <v>199</v>
+        <v>211</v>
       </c>
       <c r="C8" s="8">
         <v>100</v>
@@ -3280,22 +3289,20 @@
     </row>
     <row r="9" spans="1:10" s="2" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="10">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B9" s="15" t="s">
-        <v>156</v>
-      </c>
-      <c r="C9" s="8">
-        <v>0</v>
+        <v>208</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>209</v>
       </c>
       <c r="D9" s="8"/>
       <c r="E9" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="F9" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="G9" s="7" t="s">
+        <v>210</v>
+      </c>
+      <c r="F9" s="6"/>
+      <c r="G9" s="4" t="s">
         <v>114</v>
       </c>
       <c r="H9" s="19"/>
@@ -3303,100 +3310,102 @@
         <v>0.1</v>
       </c>
       <c r="J9" s="22">
-        <v>0.27</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="10" spans="1:10" s="2" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="10">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B10" s="15" t="s">
-        <v>198</v>
-      </c>
-      <c r="C10" s="6" t="s">
-        <v>51</v>
+        <v>156</v>
+      </c>
+      <c r="C10" s="8">
+        <v>0</v>
       </c>
       <c r="D10" s="8"/>
       <c r="E10" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="F10" s="6"/>
+        <v>41</v>
+      </c>
+      <c r="F10" s="6" t="s">
+        <v>42</v>
+      </c>
       <c r="G10" s="7" t="s">
         <v>114</v>
       </c>
-      <c r="H10" s="20"/>
+      <c r="H10" s="19"/>
       <c r="I10" s="22">
-        <v>0.19</v>
+        <v>0.1</v>
       </c>
       <c r="J10" s="22">
-        <v>1.08</v>
+        <v>0.27</v>
       </c>
     </row>
     <row r="11" spans="1:10" s="2" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="10">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B11" s="15" t="s">
-        <v>10</v>
+        <v>198</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="D11" s="8"/>
       <c r="E11" s="6" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="F11" s="6"/>
-      <c r="G11" s="4" t="s">
+      <c r="G11" s="7" t="s">
         <v>114</v>
       </c>
       <c r="H11" s="20"/>
       <c r="I11" s="22">
-        <v>0.11</v>
+        <v>0.19</v>
       </c>
       <c r="J11" s="22">
-        <v>0.63</v>
+        <v>1.08</v>
       </c>
     </row>
     <row r="12" spans="1:10" s="2" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="10">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B12" s="15" t="s">
-        <v>169</v>
+        <v>10</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="D12" s="8"/>
       <c r="E12" s="6" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="F12" s="6"/>
-      <c r="G12" s="7" t="s">
+      <c r="G12" s="4" t="s">
         <v>114</v>
       </c>
       <c r="H12" s="20"/>
       <c r="I12" s="22">
-        <v>0.08</v>
+        <v>0.11</v>
       </c>
       <c r="J12" s="22">
-        <v>0.08</v>
+        <v>0.63</v>
       </c>
     </row>
     <row r="13" spans="1:10" s="2" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="10">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B13" s="15" t="s">
-        <v>20</v>
+        <v>169</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>115</v>
+        <v>44</v>
       </c>
       <c r="D13" s="8"/>
       <c r="E13" s="6" t="s">
-        <v>33</v>
+        <v>45</v>
       </c>
       <c r="F13" s="6"/>
       <c r="G13" s="7" t="s">
@@ -3404,231 +3413,229 @@
       </c>
       <c r="H13" s="20"/>
       <c r="I13" s="22">
-        <v>0.1</v>
+        <v>0.08</v>
       </c>
       <c r="J13" s="22">
-        <v>0.22</v>
+        <v>0.08</v>
       </c>
     </row>
     <row r="14" spans="1:10" s="2" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="10">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B14" s="15" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>48</v>
+        <v>115</v>
       </c>
       <c r="D14" s="8"/>
       <c r="E14" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="F14" s="6" t="s">
-        <v>49</v>
-      </c>
+        <v>33</v>
+      </c>
+      <c r="F14" s="6"/>
       <c r="G14" s="7" t="s">
         <v>114</v>
       </c>
       <c r="H14" s="20"/>
       <c r="I14" s="22">
-        <v>1.04</v>
+        <v>0.1</v>
       </c>
       <c r="J14" s="22">
-        <v>6.31</v>
+        <v>0.22</v>
       </c>
     </row>
     <row r="15" spans="1:10" s="2" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="10">
-        <v>11</v>
-      </c>
-      <c r="B15" s="6" t="s">
-        <v>3</v>
+        <v>10</v>
+      </c>
+      <c r="B15" s="15" t="s">
+        <v>24</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="D15" s="8"/>
       <c r="E15" s="6" t="s">
-        <v>179</v>
+        <v>35</v>
       </c>
       <c r="F15" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="G15" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="G15" s="7" t="s">
         <v>114</v>
       </c>
       <c r="H15" s="20"/>
       <c r="I15" s="22">
+        <v>1.04</v>
+      </c>
+      <c r="J15" s="22">
+        <v>6.31</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" s="2" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A16" s="10">
+        <v>11</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="D16" s="8"/>
+      <c r="E16" s="6" t="s">
+        <v>179</v>
+      </c>
+      <c r="F16" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="G16" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="H16" s="20"/>
+      <c r="I16" s="22">
         <v>4</v>
       </c>
-      <c r="J15" s="22">
+      <c r="J16" s="22">
         <v>40</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="43" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A16" s="33" t="s">
+    <row r="17" spans="1:10" ht="43" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A17" s="33" t="s">
         <v>152</v>
       </c>
-      <c r="B16" s="34"/>
-      <c r="C16" s="34"/>
-      <c r="D16" s="34"/>
-      <c r="E16" s="34"/>
-      <c r="F16" s="34"/>
-      <c r="G16" s="38"/>
-      <c r="H16" s="38"/>
-      <c r="I16" s="22"/>
-      <c r="J16" s="22"/>
-    </row>
-    <row r="17" spans="1:10" s="2" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A17" s="10">
-        <v>12</v>
-      </c>
-      <c r="B17" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C17" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="D17" s="8"/>
-      <c r="E17" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="F17" s="8"/>
-      <c r="G17" s="7" t="s">
-        <v>114</v>
-      </c>
-      <c r="H17" s="20"/>
-      <c r="I17" s="22">
-        <v>0.15</v>
-      </c>
-      <c r="J17" s="22">
-        <v>1.22</v>
-      </c>
+      <c r="B17" s="34"/>
+      <c r="C17" s="34"/>
+      <c r="D17" s="34"/>
+      <c r="E17" s="34"/>
+      <c r="F17" s="34"/>
+      <c r="G17" s="38"/>
+      <c r="H17" s="38"/>
+      <c r="I17" s="22"/>
+      <c r="J17" s="22"/>
     </row>
     <row r="18" spans="1:10" s="2" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="10">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>22</v>
+        <v>9</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>23</v>
+        <v>91</v>
       </c>
       <c r="D18" s="8"/>
       <c r="E18" s="6" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="F18" s="8"/>
-      <c r="G18" s="4" t="s">
+      <c r="G18" s="7" t="s">
         <v>114</v>
       </c>
       <c r="H18" s="20"/>
       <c r="I18" s="22">
-        <v>0.1</v>
+        <v>0.15</v>
       </c>
       <c r="J18" s="22">
-        <v>0.54</v>
+        <v>1.22</v>
       </c>
     </row>
     <row r="19" spans="1:10" s="2" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="10">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>54</v>
+        <v>23</v>
       </c>
       <c r="D19" s="8"/>
       <c r="E19" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="F19" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="G19" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="F19" s="8"/>
+      <c r="G19" s="4" t="s">
         <v>114</v>
       </c>
       <c r="H19" s="20"/>
       <c r="I19" s="22">
-        <v>1.92</v>
+        <v>0.1</v>
       </c>
       <c r="J19" s="22">
-        <v>11.92</v>
+        <v>0.54</v>
       </c>
     </row>
     <row r="20" spans="1:10" s="2" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="10">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>12</v>
+        <v>54</v>
       </c>
       <c r="D20" s="8"/>
       <c r="E20" s="6" t="s">
-        <v>116</v>
+        <v>53</v>
       </c>
       <c r="F20" s="6" t="s">
-        <v>64</v>
+        <v>50</v>
       </c>
       <c r="G20" s="7" t="s">
         <v>114</v>
       </c>
       <c r="H20" s="20"/>
       <c r="I20" s="22">
-        <v>1.67</v>
+        <v>1.92</v>
       </c>
       <c r="J20" s="22">
-        <v>12.26</v>
+        <v>11.92</v>
       </c>
     </row>
     <row r="21" spans="1:10" s="2" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="10">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>157</v>
+        <v>12</v>
       </c>
       <c r="D21" s="8"/>
       <c r="E21" s="6" t="s">
-        <v>161</v>
+        <v>116</v>
       </c>
       <c r="F21" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="G21" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="G21" s="7" t="s">
         <v>114</v>
       </c>
       <c r="H21" s="20"/>
       <c r="I21" s="22">
-        <v>0.14000000000000001</v>
+        <v>1.67</v>
       </c>
       <c r="J21" s="22">
-        <v>1.08</v>
+        <v>12.26</v>
       </c>
     </row>
     <row r="22" spans="1:10" s="2" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="10">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>8</v>
+        <v>157</v>
       </c>
       <c r="D22" s="8"/>
       <c r="E22" s="6" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="F22" s="6" t="s">
         <v>55</v>
@@ -3638,121 +3645,123 @@
       </c>
       <c r="H22" s="20"/>
       <c r="I22" s="22">
-        <v>0.1</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="J22" s="22">
-        <v>0.61</v>
+        <v>1.08</v>
       </c>
     </row>
     <row r="23" spans="1:10" s="2" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="10">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>26</v>
+        <v>8</v>
       </c>
       <c r="D23" s="8"/>
       <c r="E23" s="6" t="s">
-        <v>32</v>
+        <v>162</v>
       </c>
       <c r="F23" s="6" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="G23" s="4" t="s">
         <v>114</v>
       </c>
       <c r="H23" s="20"/>
       <c r="I23" s="22">
-        <v>0.13</v>
+        <v>0.1</v>
       </c>
       <c r="J23" s="22">
-        <v>0.8</v>
+        <v>0.61</v>
       </c>
     </row>
     <row r="24" spans="1:10" s="2" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="10">
+        <v>18</v>
+      </c>
+      <c r="B24" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="B24" s="6" t="s">
-        <v>57</v>
-      </c>
       <c r="C24" s="6" t="s">
-        <v>56</v>
+        <v>26</v>
       </c>
       <c r="D24" s="8"/>
       <c r="E24" s="6" t="s">
-        <v>58</v>
+        <v>32</v>
       </c>
       <c r="F24" s="6" t="s">
-        <v>108</v>
+        <v>50</v>
       </c>
       <c r="G24" s="4" t="s">
         <v>114</v>
       </c>
       <c r="H24" s="20"/>
       <c r="I24" s="22">
+        <v>0.13</v>
+      </c>
+      <c r="J24" s="22">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" s="2" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A25" s="10">
+        <v>19</v>
+      </c>
+      <c r="B25" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="C25" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="D25" s="8"/>
+      <c r="E25" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="F25" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="G25" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="H25" s="20"/>
+      <c r="I25" s="22">
         <v>0.89</v>
       </c>
-      <c r="J24" s="22">
+      <c r="J25" s="22">
         <v>7.55</v>
       </c>
     </row>
-    <row r="25" spans="1:10" ht="41" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A25" s="33" t="s">
+    <row r="26" spans="1:10" ht="41" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A26" s="33" t="s">
         <v>180</v>
       </c>
-      <c r="B25" s="34"/>
-      <c r="C25" s="34"/>
-      <c r="D25" s="34"/>
-      <c r="E25" s="34"/>
-      <c r="F25" s="34"/>
-      <c r="G25" s="35"/>
-      <c r="H25" s="35"/>
-      <c r="I25" s="22"/>
-      <c r="J25" s="22"/>
-    </row>
-    <row r="26" spans="1:10" s="2" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A26" s="10">
-        <v>20</v>
-      </c>
-      <c r="B26" s="6" t="s">
-        <v>200</v>
-      </c>
-      <c r="C26" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="D26" s="8"/>
-      <c r="E26" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="F26" s="6"/>
-      <c r="G26" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="H26" s="20"/>
-      <c r="I26" s="22">
-        <v>0.1</v>
-      </c>
-      <c r="J26" s="22">
-        <v>0.14000000000000001</v>
-      </c>
+      <c r="B26" s="34"/>
+      <c r="C26" s="34"/>
+      <c r="D26" s="34"/>
+      <c r="E26" s="34"/>
+      <c r="F26" s="34"/>
+      <c r="G26" s="35"/>
+      <c r="H26" s="35"/>
+      <c r="I26" s="22"/>
+      <c r="J26" s="22"/>
     </row>
     <row r="27" spans="1:10" s="2" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="10">
+        <v>20</v>
+      </c>
+      <c r="B27" s="6" t="s">
+        <v>199</v>
+      </c>
+      <c r="C27" s="6" t="s">
         <v>21</v>
-      </c>
-      <c r="B27" s="6" t="s">
-        <v>158</v>
-      </c>
-      <c r="C27" s="6" t="s">
-        <v>160</v>
       </c>
       <c r="D27" s="8"/>
       <c r="E27" s="6" t="s">
-        <v>159</v>
+        <v>59</v>
       </c>
       <c r="F27" s="6"/>
       <c r="G27" s="4" t="s">
@@ -3763,22 +3772,22 @@
         <v>0.1</v>
       </c>
       <c r="J27" s="22">
-        <v>0.12</v>
+        <v>0.14000000000000001</v>
       </c>
     </row>
     <row r="28" spans="1:10" s="2" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" s="10">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>5</v>
+        <v>158</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>60</v>
+        <v>160</v>
       </c>
       <c r="D28" s="8"/>
       <c r="E28" s="6" t="s">
-        <v>61</v>
+        <v>159</v>
       </c>
       <c r="F28" s="6"/>
       <c r="G28" s="4" t="s">
@@ -3794,17 +3803,17 @@
     </row>
     <row r="29" spans="1:10" s="2" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29" s="10">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>163</v>
+        <v>5</v>
       </c>
       <c r="C29" s="6" t="s">
-        <v>1</v>
+        <v>60</v>
       </c>
       <c r="D29" s="8"/>
       <c r="E29" s="6" t="s">
-        <v>117</v>
+        <v>61</v>
       </c>
       <c r="F29" s="6"/>
       <c r="G29" s="4" t="s">
@@ -3812,312 +3821,308 @@
       </c>
       <c r="H29" s="20"/>
       <c r="I29" s="22">
-        <v>0.13</v>
+        <v>0.1</v>
       </c>
       <c r="J29" s="22">
-        <v>0.16</v>
+        <v>0.12</v>
       </c>
     </row>
     <row r="30" spans="1:10" s="2" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" s="10">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C30" s="6" t="s">
-        <v>63</v>
+        <v>1</v>
       </c>
       <c r="D30" s="8"/>
       <c r="E30" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="F30" s="8"/>
+        <v>117</v>
+      </c>
+      <c r="F30" s="6"/>
       <c r="G30" s="4" t="s">
         <v>114</v>
       </c>
       <c r="H30" s="20"/>
       <c r="I30" s="22">
-        <v>0.1</v>
+        <v>0.13</v>
       </c>
       <c r="J30" s="22">
-        <v>0.49</v>
+        <v>0.16</v>
       </c>
     </row>
     <row r="31" spans="1:10" s="2" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A31" s="10">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>17</v>
+        <v>164</v>
       </c>
       <c r="C31" s="6" t="s">
-        <v>18</v>
+        <v>63</v>
       </c>
       <c r="D31" s="8"/>
       <c r="E31" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="F31" s="8" t="s">
-        <v>69</v>
-      </c>
+        <v>62</v>
+      </c>
+      <c r="F31" s="8"/>
       <c r="G31" s="4" t="s">
         <v>114</v>
       </c>
       <c r="H31" s="20"/>
       <c r="I31" s="22">
-        <v>0.13</v>
+        <v>0.1</v>
       </c>
       <c r="J31" s="22">
-        <v>0.73</v>
+        <v>0.49</v>
       </c>
     </row>
     <row r="32" spans="1:10" s="2" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A32" s="10">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B32" s="6" t="s">
-        <v>65</v>
+        <v>17</v>
       </c>
       <c r="C32" s="6" t="s">
-        <v>66</v>
+        <v>18</v>
       </c>
       <c r="D32" s="8"/>
       <c r="E32" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="F32" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="G32" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="H32" s="20"/>
+      <c r="I32" s="22">
+        <v>0.13</v>
+      </c>
+      <c r="J32" s="22">
+        <v>0.73</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" s="2" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A33" s="10">
+        <v>27</v>
+      </c>
+      <c r="B33" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="C33" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="D33" s="8"/>
+      <c r="E33" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="F32" s="6" t="s">
+      <c r="F33" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="G32" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="H32" s="18" t="s">
-        <v>114</v>
-      </c>
-      <c r="I32" s="22">
+      <c r="G33" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="H33" s="18" t="s">
+        <v>114</v>
+      </c>
+      <c r="I33" s="22">
         <v>2.48</v>
       </c>
-      <c r="J32" s="22">
+      <c r="J33" s="22">
         <v>21.07</v>
       </c>
     </row>
-    <row r="33" spans="1:10" ht="32" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A33" s="33" t="s">
+    <row r="34" spans="1:10" ht="32" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A34" s="33" t="s">
         <v>150</v>
       </c>
-      <c r="B33" s="34"/>
-      <c r="C33" s="34"/>
-      <c r="D33" s="34"/>
-      <c r="E33" s="34"/>
-      <c r="F33" s="34"/>
-      <c r="G33" s="35"/>
-      <c r="H33" s="35"/>
-      <c r="I33" s="22"/>
-      <c r="J33" s="22"/>
-    </row>
-    <row r="34" spans="1:10" s="2" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A34" s="10">
-        <v>28</v>
-      </c>
-      <c r="B34" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="C34" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="D34" s="8"/>
-      <c r="E34" s="6" t="s">
-        <v>147</v>
-      </c>
-      <c r="F34" s="9" t="s">
-        <v>72</v>
-      </c>
-      <c r="G34" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="H34" s="18" t="s">
-        <v>114</v>
-      </c>
-      <c r="I34" s="22">
-        <v>0.33</v>
-      </c>
-      <c r="J34" s="22">
-        <v>2.82</v>
-      </c>
+      <c r="B34" s="34"/>
+      <c r="C34" s="34"/>
+      <c r="D34" s="34"/>
+      <c r="E34" s="34"/>
+      <c r="F34" s="34"/>
+      <c r="G34" s="35"/>
+      <c r="H34" s="35"/>
+      <c r="I34" s="22"/>
+      <c r="J34" s="22"/>
     </row>
     <row r="35" spans="1:10" s="2" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A35" s="10">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B35" s="6" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C35" s="6" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="D35" s="8"/>
       <c r="E35" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="F35" s="6" t="s">
+        <v>147</v>
+      </c>
+      <c r="F35" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="G35" s="4"/>
+      <c r="G35" s="4" t="s">
+        <v>114</v>
+      </c>
       <c r="H35" s="18" t="s">
         <v>114</v>
       </c>
       <c r="I35" s="22">
-        <v>0.45</v>
+        <v>0.33</v>
       </c>
       <c r="J35" s="22">
-        <v>3.83</v>
+        <v>2.82</v>
       </c>
     </row>
     <row r="36" spans="1:10" s="2" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A36" s="10">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B36" s="6" t="s">
-        <v>4</v>
+        <v>73</v>
       </c>
       <c r="C36" s="6" t="s">
-        <v>4</v>
+        <v>74</v>
       </c>
       <c r="D36" s="8"/>
       <c r="E36" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="F36" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="G36" s="4"/>
+      <c r="H36" s="18" t="s">
+        <v>114</v>
+      </c>
+      <c r="I36" s="22">
+        <v>0.45</v>
+      </c>
+      <c r="J36" s="22">
+        <v>3.83</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" s="2" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A37" s="10">
+        <v>30</v>
+      </c>
+      <c r="B37" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C37" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D37" s="8"/>
+      <c r="E37" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="F36" s="11" t="s">
+      <c r="F37" s="11" t="s">
         <v>76</v>
       </c>
-      <c r="G36" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="H36" s="18" t="s">
-        <v>114</v>
-      </c>
-      <c r="I36" s="24">
+      <c r="G37" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="H37" s="18" t="s">
+        <v>114</v>
+      </c>
+      <c r="I37" s="24">
         <f>6.89/10</f>
         <v>0.68899999999999995</v>
       </c>
-      <c r="J36" s="22">
+      <c r="J37" s="22">
         <v>6.89</v>
       </c>
     </row>
-    <row r="37" spans="1:10" s="2" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A37" s="10">
+    <row r="38" spans="1:10" s="2" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A38" s="10">
         <v>31</v>
       </c>
-      <c r="B37" s="6" t="s">
+      <c r="B38" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="C37" s="6" t="s">
+      <c r="C38" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="D37" s="8"/>
-      <c r="E37" s="6" t="s">
+      <c r="D38" s="8"/>
+      <c r="E38" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="F37" s="12" t="s">
-        <v>201</v>
-      </c>
-      <c r="G37" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="H37" s="18" t="s">
-        <v>114</v>
-      </c>
-      <c r="I37" s="22">
+      <c r="F38" s="12" t="s">
+        <v>200</v>
+      </c>
+      <c r="G38" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="H38" s="18" t="s">
+        <v>114</v>
+      </c>
+      <c r="I38" s="22">
         <f>7.39/5</f>
         <v>1.478</v>
       </c>
-      <c r="J37" s="22">
+      <c r="J38" s="22">
         <f>7.39*2</f>
         <v>14.78</v>
       </c>
     </row>
-    <row r="38" spans="1:10" s="2" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A38" s="10">
+    <row r="39" spans="1:10" s="2" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A39" s="10">
         <v>32</v>
       </c>
-      <c r="B38" s="6" t="s">
+      <c r="B39" s="6" t="s">
         <v>167</v>
       </c>
-      <c r="C38" s="6" t="s">
+      <c r="C39" s="6" t="s">
         <v>165</v>
       </c>
-      <c r="D38" s="8"/>
-      <c r="E38" s="6" t="s">
+      <c r="D39" s="8"/>
+      <c r="E39" s="6" t="s">
         <v>166</v>
       </c>
-      <c r="F38" s="12" t="s">
-        <v>202</v>
-      </c>
-      <c r="G38" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="H38" s="20"/>
-      <c r="I38" s="22">
+      <c r="F39" s="12" t="s">
+        <v>201</v>
+      </c>
+      <c r="G39" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="H39" s="20"/>
+      <c r="I39" s="22">
         <v>6.99</v>
       </c>
-      <c r="J38" s="22">
+      <c r="J39" s="22">
         <f>3.663333333*10</f>
         <v>36.633333329999999</v>
       </c>
     </row>
-    <row r="39" spans="1:10" s="2" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A39" s="10">
-        <v>33</v>
-      </c>
-      <c r="B39" s="6" t="s">
-        <v>203</v>
-      </c>
-      <c r="C39" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="D39" s="8"/>
-      <c r="E39" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="F39" s="12" t="s">
-        <v>82</v>
-      </c>
-      <c r="G39" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="H39" s="20"/>
-      <c r="I39" s="24">
-        <f>6.99/100</f>
-        <v>6.9900000000000004E-2</v>
-      </c>
-      <c r="J39" s="22">
-        <f>6.99/10</f>
-        <v>0.69900000000000007</v>
-      </c>
-    </row>
     <row r="40" spans="1:10" s="2" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A40" s="10">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B40" s="6" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="C40" s="6" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="D40" s="8"/>
-      <c r="E40" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="F40" s="13" t="s">
-        <v>85</v>
+      <c r="E40" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="F40" s="12" t="s">
+        <v>82</v>
       </c>
       <c r="G40" s="4" t="s">
         <v>114</v>
       </c>
       <c r="H40" s="20"/>
-      <c r="I40" s="22">
+      <c r="I40" s="24">
         <f>6.99/100</f>
         <v>6.9900000000000004E-2</v>
       </c>
@@ -4128,119 +4133,123 @@
     </row>
     <row r="41" spans="1:10" s="2" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A41" s="10">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B41" s="6" t="s">
-        <v>86</v>
+        <v>203</v>
       </c>
       <c r="C41" s="6" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="D41" s="8"/>
-      <c r="E41" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="F41" s="12" t="s">
-        <v>92</v>
+      <c r="E41" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="F41" s="13" t="s">
+        <v>85</v>
       </c>
       <c r="G41" s="4" t="s">
         <v>114</v>
       </c>
-      <c r="H41" s="18" t="s">
-        <v>114</v>
-      </c>
+      <c r="H41" s="20"/>
       <c r="I41" s="22">
-        <v>5</v>
+        <f>6.99/100</f>
+        <v>6.9900000000000004E-2</v>
       </c>
       <c r="J41" s="22">
-        <v>28</v>
+        <f>6.99/10</f>
+        <v>0.69900000000000007</v>
       </c>
     </row>
     <row r="42" spans="1:10" s="2" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A42" s="10">
+        <v>35</v>
+      </c>
+      <c r="B42" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="C42" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="D42" s="8"/>
+      <c r="E42" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="F42" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="G42" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="H42" s="18" t="s">
+        <v>114</v>
+      </c>
+      <c r="I42" s="22">
+        <v>5</v>
+      </c>
+      <c r="J42" s="22">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" s="2" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A43" s="10">
         <v>36</v>
       </c>
-      <c r="B42" s="6" t="s">
+      <c r="B43" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="C42" s="6" t="s">
+      <c r="C43" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="D42" s="8"/>
-      <c r="E42" s="8" t="s">
+      <c r="D43" s="8"/>
+      <c r="E43" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="F42" s="11" t="s">
+      <c r="F43" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="G42" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="H42" s="18" t="s">
-        <v>114</v>
-      </c>
-      <c r="I42" s="22">
+      <c r="G43" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="H43" s="18" t="s">
+        <v>114</v>
+      </c>
+      <c r="I43" s="22">
         <f>7.29/6</f>
         <v>1.2150000000000001</v>
       </c>
-      <c r="J42" s="22">
-        <f>I42*10</f>
+      <c r="J43" s="22">
+        <f>I43*10</f>
         <v>12.15</v>
       </c>
     </row>
-    <row r="43" spans="1:10" ht="54" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A43" s="33" t="s">
+    <row r="44" spans="1:10" ht="54" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A44" s="33" t="s">
         <v>93</v>
       </c>
-      <c r="B43" s="34"/>
-      <c r="C43" s="34"/>
-      <c r="D43" s="34"/>
-      <c r="E43" s="34"/>
-      <c r="F43" s="34"/>
-      <c r="G43" s="35"/>
-      <c r="H43" s="35"/>
-      <c r="I43" s="22"/>
-      <c r="J43" s="22"/>
-    </row>
-    <row r="44" spans="1:10" s="2" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A44" s="14">
-        <v>37</v>
-      </c>
-      <c r="B44" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="C44" s="15" t="s">
-        <v>94</v>
-      </c>
-      <c r="D44" s="11"/>
-      <c r="E44" s="15" t="s">
-        <v>95</v>
-      </c>
-      <c r="F44" s="13"/>
-      <c r="G44" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="H44" s="20"/>
-      <c r="I44" s="22">
-        <v>0.11</v>
-      </c>
-      <c r="J44" s="22">
-        <v>0.61</v>
-      </c>
+      <c r="B44" s="34"/>
+      <c r="C44" s="34"/>
+      <c r="D44" s="34"/>
+      <c r="E44" s="34"/>
+      <c r="F44" s="34"/>
+      <c r="G44" s="35"/>
+      <c r="H44" s="35"/>
+      <c r="I44" s="22"/>
+      <c r="J44" s="22"/>
     </row>
     <row r="45" spans="1:10" s="2" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A45" s="14">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B45" s="15" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C45" s="15" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D45" s="11"/>
       <c r="E45" s="15" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="F45" s="13"/>
       <c r="G45" s="4" t="s">
@@ -4248,28 +4257,28 @@
       </c>
       <c r="H45" s="20"/>
       <c r="I45" s="22">
-        <v>0.08</v>
+        <v>0.11</v>
       </c>
       <c r="J45" s="22">
-        <v>0.11</v>
+        <v>0.61</v>
       </c>
     </row>
     <row r="46" spans="1:10" s="2" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A46" s="14">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B46" s="15" t="s">
-        <v>168</v>
-      </c>
-      <c r="C46" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="D46" s="8"/>
-      <c r="E46" s="6" t="s">
-        <v>45</v>
+        <v>15</v>
+      </c>
+      <c r="C46" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="D46" s="11"/>
+      <c r="E46" s="15" t="s">
+        <v>97</v>
       </c>
       <c r="F46" s="13"/>
-      <c r="G46" s="7" t="s">
+      <c r="G46" s="4" t="s">
         <v>114</v>
       </c>
       <c r="H46" s="20"/>
@@ -4277,689 +4286,716 @@
         <v>0.08</v>
       </c>
       <c r="J46" s="22">
-        <v>0.08</v>
+        <v>0.11</v>
       </c>
     </row>
     <row r="47" spans="1:10" s="2" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A47" s="14">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B47" s="15" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C47" s="6" t="s">
-        <v>171</v>
+        <v>44</v>
       </c>
       <c r="D47" s="8"/>
       <c r="E47" s="6" t="s">
-        <v>172</v>
+        <v>45</v>
       </c>
       <c r="F47" s="13"/>
-      <c r="G47" s="4" t="s">
+      <c r="G47" s="7" t="s">
         <v>114</v>
       </c>
       <c r="H47" s="20"/>
       <c r="I47" s="22">
-        <v>0.11</v>
+        <v>0.08</v>
       </c>
       <c r="J47" s="22">
-        <v>0.35</v>
+        <v>0.08</v>
       </c>
     </row>
     <row r="48" spans="1:10" s="2" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A48" s="14">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B48" s="15" t="s">
-        <v>181</v>
+        <v>170</v>
       </c>
       <c r="C48" s="6" t="s">
-        <v>182</v>
+        <v>171</v>
       </c>
       <c r="D48" s="8"/>
       <c r="E48" s="6" t="s">
-        <v>40</v>
+        <v>172</v>
       </c>
       <c r="F48" s="13"/>
-      <c r="G48" s="7" t="s">
+      <c r="G48" s="4" t="s">
         <v>114</v>
       </c>
       <c r="H48" s="20"/>
       <c r="I48" s="22">
-        <v>0.1</v>
+        <v>0.11</v>
       </c>
       <c r="J48" s="22">
-        <v>0.25</v>
+        <v>0.35</v>
       </c>
     </row>
     <row r="49" spans="1:10" s="2" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A49" s="14">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B49" s="15" t="s">
-        <v>205</v>
-      </c>
-      <c r="C49" s="15" t="s">
-        <v>98</v>
-      </c>
-      <c r="D49" s="11"/>
-      <c r="E49" s="15" t="s">
-        <v>105</v>
-      </c>
-      <c r="F49" s="12" t="s">
-        <v>100</v>
-      </c>
-      <c r="G49" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="C49" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="D49" s="8"/>
+      <c r="E49" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="F49" s="13"/>
+      <c r="G49" s="7" t="s">
         <v>114</v>
       </c>
       <c r="H49" s="20"/>
       <c r="I49" s="22">
-        <v>0.53</v>
+        <v>0.1</v>
       </c>
       <c r="J49" s="22">
-        <v>4.51</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="50" spans="1:10" s="2" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A50" s="14">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B50" s="15" t="s">
-        <v>2</v>
+        <v>204</v>
       </c>
       <c r="C50" s="15" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D50" s="11"/>
       <c r="E50" s="15" t="s">
-        <v>187</v>
+        <v>105</v>
       </c>
       <c r="F50" s="12" t="s">
-        <v>206</v>
+        <v>100</v>
       </c>
       <c r="G50" s="4" t="s">
         <v>114</v>
       </c>
       <c r="H50" s="20"/>
       <c r="I50" s="22">
-        <v>28.41</v>
+        <v>0.53</v>
       </c>
       <c r="J50" s="22">
-        <v>251.47</v>
+        <v>4.51</v>
       </c>
     </row>
     <row r="51" spans="1:10" s="2" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A51" s="14">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B51" s="15" t="s">
-        <v>103</v>
+        <v>2</v>
       </c>
       <c r="C51" s="15" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D51" s="11"/>
       <c r="E51" s="15" t="s">
-        <v>102</v>
-      </c>
-      <c r="F51" s="11" t="s">
-        <v>118</v>
+        <v>187</v>
+      </c>
+      <c r="F51" s="12" t="s">
+        <v>205</v>
       </c>
       <c r="G51" s="4" t="s">
         <v>114</v>
       </c>
       <c r="H51" s="20"/>
       <c r="I51" s="22">
-        <v>0.7</v>
+        <v>28.41</v>
       </c>
       <c r="J51" s="22">
-        <v>5.9</v>
+        <v>251.47</v>
       </c>
     </row>
     <row r="52" spans="1:10" s="2" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A52" s="14">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B52" s="15" t="s">
-        <v>208</v>
+        <v>103</v>
       </c>
       <c r="C52" s="15" t="s">
         <v>101</v>
       </c>
       <c r="D52" s="11"/>
       <c r="E52" s="15" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="F52" s="11" t="s">
-        <v>207</v>
+        <v>118</v>
       </c>
       <c r="G52" s="4" t="s">
         <v>114</v>
       </c>
       <c r="H52" s="20"/>
       <c r="I52" s="22">
+        <v>0.7</v>
+      </c>
+      <c r="J52" s="22">
+        <v>5.9</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" s="2" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A53" s="14">
+        <v>45</v>
+      </c>
+      <c r="B53" s="15" t="s">
+        <v>207</v>
+      </c>
+      <c r="C53" s="15" t="s">
+        <v>101</v>
+      </c>
+      <c r="D53" s="11"/>
+      <c r="E53" s="15" t="s">
+        <v>106</v>
+      </c>
+      <c r="F53" s="11" t="s">
+        <v>206</v>
+      </c>
+      <c r="G53" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="H53" s="20"/>
+      <c r="I53" s="22">
         <f>6.79/100</f>
         <v>6.7900000000000002E-2</v>
       </c>
-      <c r="J52" s="22">
+      <c r="J53" s="22">
         <f>6.79/10</f>
         <v>0.67900000000000005</v>
       </c>
     </row>
-    <row r="53" spans="1:10" ht="32" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A53" s="36" t="s">
+    <row r="54" spans="1:10" ht="32" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A54" s="36" t="s">
         <v>104</v>
       </c>
-      <c r="B53" s="37"/>
-      <c r="C53" s="37"/>
-      <c r="D53" s="37"/>
-      <c r="E53" s="37"/>
-      <c r="F53" s="37"/>
-      <c r="G53" s="38"/>
-      <c r="H53" s="38"/>
-      <c r="I53" s="22"/>
-      <c r="J53" s="22"/>
-    </row>
-    <row r="54" spans="1:10" s="2" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A54" s="14">
+      <c r="B54" s="37"/>
+      <c r="C54" s="37"/>
+      <c r="D54" s="37"/>
+      <c r="E54" s="37"/>
+      <c r="F54" s="37"/>
+      <c r="G54" s="38"/>
+      <c r="H54" s="38"/>
+      <c r="I54" s="22"/>
+      <c r="J54" s="22"/>
+    </row>
+    <row r="55" spans="1:10" s="2" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A55" s="14">
         <v>46</v>
       </c>
-      <c r="B54" s="15" t="s">
+      <c r="B55" s="15" t="s">
         <v>119</v>
       </c>
-      <c r="C54" s="15" t="s">
+      <c r="C55" s="15" t="s">
         <v>109</v>
       </c>
-      <c r="D54" s="11"/>
-      <c r="E54" s="15" t="s">
+      <c r="D55" s="11"/>
+      <c r="E55" s="15" t="s">
         <v>183</v>
       </c>
-      <c r="F54" s="11"/>
-      <c r="G54" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="H54" s="20"/>
-      <c r="I54" s="22">
-        <v>19</v>
-      </c>
-      <c r="J54" s="22">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="55" spans="1:10" s="2" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A55" s="10">
-        <v>47</v>
-      </c>
-      <c r="B55" s="6" t="s">
-        <v>112</v>
-      </c>
-      <c r="C55" s="6" t="s">
-        <v>129</v>
-      </c>
-      <c r="D55" s="8"/>
-      <c r="E55" s="6" t="s">
-        <v>151</v>
-      </c>
-      <c r="F55" s="3" t="s">
-        <v>173</v>
-      </c>
+      <c r="F55" s="11"/>
       <c r="G55" s="4" t="s">
         <v>114</v>
       </c>
       <c r="H55" s="20"/>
       <c r="I55" s="22">
+        <v>19</v>
+      </c>
+      <c r="J55" s="22">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" s="2" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A56" s="10">
+        <v>47</v>
+      </c>
+      <c r="B56" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="C56" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="D56" s="8"/>
+      <c r="E56" s="6" t="s">
+        <v>151</v>
+      </c>
+      <c r="F56" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="G56" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="H56" s="20"/>
+      <c r="I56" s="22">
         <v>0.1</v>
       </c>
-      <c r="J55" s="22">
+      <c r="J56" s="22">
         <v>0.1</v>
       </c>
     </row>
-    <row r="56" spans="1:10" s="2" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A56" s="14">
+    <row r="57" spans="1:10" s="2" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A57" s="14">
         <v>48</v>
       </c>
-      <c r="B56" s="6" t="s">
+      <c r="B57" s="6" t="s">
         <v>111</v>
       </c>
-      <c r="C56" s="6" t="s">
+      <c r="C57" s="6" t="s">
         <v>139</v>
       </c>
-      <c r="D56" s="8"/>
-      <c r="E56" s="6"/>
-      <c r="F56" s="6" t="s">
+      <c r="D57" s="8"/>
+      <c r="E57" s="6"/>
+      <c r="F57" s="6" t="s">
         <v>174</v>
       </c>
-      <c r="G56" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="H56" s="21"/>
-      <c r="I56" s="22">
+      <c r="G57" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="H57" s="21"/>
+      <c r="I57" s="22">
         <v>9.9499999999999993</v>
       </c>
-      <c r="J56" s="22">
+      <c r="J57" s="22">
         <v>9.9499999999999993</v>
       </c>
     </row>
-    <row r="57" spans="1:10" s="2" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A57" s="10">
+    <row r="58" spans="1:10" s="2" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A58" s="10">
         <v>49</v>
       </c>
-      <c r="B57" s="6" t="s">
+      <c r="B58" s="6" t="s">
         <v>110</v>
       </c>
-      <c r="C57" s="6" t="s">
+      <c r="C58" s="6" t="s">
         <v>127</v>
       </c>
-      <c r="D57" s="8"/>
-      <c r="E57" s="8" t="s">
+      <c r="D58" s="8"/>
+      <c r="E58" s="8" t="s">
         <v>175</v>
       </c>
-      <c r="F57" s="8" t="s">
+      <c r="F58" s="8" t="s">
         <v>128</v>
       </c>
-      <c r="G57" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="H57" s="20"/>
-      <c r="I57" s="24">
+      <c r="G58" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="H58" s="20"/>
+      <c r="I58" s="24">
         <f>12.69/10</f>
         <v>1.2689999999999999</v>
       </c>
-      <c r="J57" s="22">
+      <c r="J58" s="22">
         <v>12.69</v>
       </c>
     </row>
-    <row r="58" spans="1:10" s="2" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A58" s="14">
+    <row r="59" spans="1:10" s="2" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A59" s="14">
         <v>50</v>
       </c>
-      <c r="B58" s="6" t="s">
+      <c r="B59" s="6" t="s">
         <v>145</v>
       </c>
-      <c r="C58" s="6" t="s">
+      <c r="C59" s="6" t="s">
         <v>185</v>
       </c>
-      <c r="D58" s="8"/>
-      <c r="E58" s="8" t="s">
+      <c r="D59" s="8"/>
+      <c r="E59" s="8" t="s">
         <v>184</v>
       </c>
-      <c r="F58" s="8" t="s">
+      <c r="F59" s="8" t="s">
         <v>107</v>
       </c>
-      <c r="G58" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="H58" s="20"/>
-      <c r="I58" s="24">
+      <c r="G59" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="H59" s="20"/>
+      <c r="I59" s="24">
         <f>2.65/100</f>
         <v>2.6499999999999999E-2</v>
       </c>
-      <c r="J58" s="22">
-        <f>I58*10</f>
+      <c r="J59" s="22">
+        <f>I59*10</f>
         <v>0.26500000000000001</v>
       </c>
     </row>
-    <row r="59" spans="1:10" s="2" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A59" s="10">
+    <row r="60" spans="1:10" s="2" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A60" s="10">
         <v>51</v>
       </c>
-      <c r="B59" s="6" t="s">
+      <c r="B60" s="6" t="s">
         <v>135</v>
       </c>
-      <c r="C59" s="6" t="s">
+      <c r="C60" s="6" t="s">
         <v>136</v>
-      </c>
-      <c r="D59" s="8"/>
-      <c r="E59" s="6" t="s">
-        <v>137</v>
-      </c>
-      <c r="F59" s="3" t="s">
-        <v>138</v>
-      </c>
-      <c r="G59" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="H59" s="20"/>
-      <c r="I59" s="22">
-        <v>1.69</v>
-      </c>
-      <c r="J59" s="22">
-        <v>16.920000000000002</v>
-      </c>
-    </row>
-    <row r="60" spans="1:10" s="2" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A60" s="14">
-        <v>52</v>
-      </c>
-      <c r="B60" s="6" t="s">
-        <v>189</v>
-      </c>
-      <c r="C60" s="6" t="s">
-        <v>124</v>
       </c>
       <c r="D60" s="8"/>
       <c r="E60" s="6" t="s">
+        <v>137</v>
+      </c>
+      <c r="F60" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="G60" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="H60" s="20"/>
+      <c r="I60" s="22">
+        <v>1.69</v>
+      </c>
+      <c r="J60" s="22">
+        <v>16.920000000000002</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10" s="2" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A61" s="14">
+        <v>52</v>
+      </c>
+      <c r="B61" s="6" t="s">
+        <v>189</v>
+      </c>
+      <c r="C61" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="D61" s="8"/>
+      <c r="E61" s="6" t="s">
         <v>125</v>
       </c>
-      <c r="F60" s="3" t="s">
+      <c r="F61" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="G60" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="H60" s="18" t="s">
-        <v>114</v>
-      </c>
-      <c r="I60" s="24">
+      <c r="G61" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="H61" s="18" t="s">
+        <v>114</v>
+      </c>
+      <c r="I61" s="24">
         <f>8.89/6</f>
         <v>1.4816666666666667</v>
       </c>
-      <c r="J60" s="22">
+      <c r="J61" s="22">
         <f>8.89</f>
         <v>8.89</v>
       </c>
     </row>
-    <row r="61" spans="1:10" s="2" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A61" s="10">
+    <row r="62" spans="1:10" s="2" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A62" s="10">
         <v>53</v>
       </c>
-      <c r="B61" s="6" t="s">
+      <c r="B62" s="6" t="s">
         <v>121</v>
       </c>
-      <c r="C61" s="6" t="s">
+      <c r="C62" s="6" t="s">
         <v>122</v>
-      </c>
-      <c r="D61" s="8"/>
-      <c r="E61" s="6" t="s">
-        <v>120</v>
-      </c>
-      <c r="F61" s="3" t="s">
-        <v>188</v>
-      </c>
-      <c r="G61" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="H61" s="21"/>
-      <c r="I61" s="22">
-        <v>9</v>
-      </c>
-      <c r="J61" s="22">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="62" spans="1:10" s="2" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A62" s="14">
-        <v>54</v>
-      </c>
-      <c r="B62" s="6" t="s">
-        <v>123</v>
-      </c>
-      <c r="C62" s="6" t="s">
-        <v>142</v>
       </c>
       <c r="D62" s="8"/>
       <c r="E62" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="F62" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="G62" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="H62" s="21"/>
+      <c r="I62" s="22">
+        <v>9</v>
+      </c>
+      <c r="J62" s="22">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10" s="2" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A63" s="14">
+        <v>54</v>
+      </c>
+      <c r="B63" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="C63" s="6" t="s">
+        <v>142</v>
+      </c>
+      <c r="D63" s="8"/>
+      <c r="E63" s="6" t="s">
         <v>176</v>
       </c>
-      <c r="F62" s="3"/>
-      <c r="G62" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="H62" s="18" t="s">
-        <v>114</v>
-      </c>
-      <c r="I62" s="24">
+      <c r="F63" s="3"/>
+      <c r="G63" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="H63" s="18" t="s">
+        <v>114</v>
+      </c>
+      <c r="I63" s="24">
         <f>3.99/100</f>
         <v>3.9900000000000005E-2</v>
       </c>
-      <c r="J62" s="22">
-        <f>100*I62</f>
+      <c r="J63" s="22">
+        <f>100*I63</f>
         <v>3.9900000000000007</v>
       </c>
     </row>
-    <row r="63" spans="1:10" s="2" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A63" s="10">
+    <row r="64" spans="1:10" s="2" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A64" s="10">
         <v>55</v>
       </c>
-      <c r="B63" s="6" t="s">
+      <c r="B64" s="6" t="s">
         <v>131</v>
       </c>
-      <c r="C63" s="6" t="s">
+      <c r="C64" s="6" t="s">
         <v>130</v>
       </c>
-      <c r="D63" s="8"/>
-      <c r="E63" s="6" t="s">
+      <c r="D64" s="8"/>
+      <c r="E64" s="6" t="s">
         <v>130</v>
       </c>
-      <c r="F63" s="3"/>
-      <c r="G63" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="H63" s="18" t="s">
-        <v>114</v>
-      </c>
-      <c r="I63" s="22">
+      <c r="F64" s="3"/>
+      <c r="G64" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="H64" s="18" t="s">
+        <v>114</v>
+      </c>
+      <c r="I64" s="22">
         <f>6.09/20</f>
         <v>0.30449999999999999</v>
       </c>
-      <c r="J63" s="22">
-        <f>I63*10</f>
+      <c r="J64" s="22">
+        <f>I64*10</f>
         <v>3.0449999999999999</v>
       </c>
     </row>
-    <row r="64" spans="1:10" s="2" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A64" s="14">
+    <row r="65" spans="1:10" s="2" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A65" s="14">
         <v>56</v>
       </c>
-      <c r="B64" s="6" t="s">
+      <c r="B65" s="6" t="s">
         <v>132</v>
       </c>
-      <c r="C64" s="6" t="s">
+      <c r="C65" s="6" t="s">
         <v>133</v>
       </c>
-      <c r="D64" s="8"/>
-      <c r="E64" s="6" t="s">
+      <c r="D65" s="8"/>
+      <c r="E65" s="6" t="s">
         <v>133</v>
       </c>
-      <c r="F64" s="3"/>
-      <c r="G64" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="H64" s="18" t="s">
-        <v>114</v>
-      </c>
-      <c r="I64" s="22">
+      <c r="F65" s="3"/>
+      <c r="G65" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="H65" s="18" t="s">
+        <v>114</v>
+      </c>
+      <c r="I65" s="22">
         <f>11.39/100</f>
         <v>0.1139</v>
       </c>
-      <c r="J64" s="22">
-        <f>I64*10</f>
+      <c r="J65" s="22">
+        <f>I65*10</f>
         <v>1.139</v>
       </c>
     </row>
-    <row r="65" spans="1:10" s="2" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A65" s="10">
+    <row r="66" spans="1:10" s="2" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A66" s="10">
         <v>57</v>
       </c>
-      <c r="B65" s="6" t="s">
+      <c r="B66" s="6" t="s">
         <v>143</v>
       </c>
-      <c r="C65" s="6" t="s">
+      <c r="C66" s="6" t="s">
         <v>144</v>
-      </c>
-      <c r="D65" s="8"/>
-      <c r="E65" s="6" t="s">
-        <v>141</v>
-      </c>
-      <c r="F65" s="3" t="s">
-        <v>177</v>
-      </c>
-      <c r="G65" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="H65" s="21"/>
-      <c r="I65" s="22">
-        <v>1</v>
-      </c>
-      <c r="J65" s="22">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="66" spans="1:10" s="2" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A66" s="14">
-        <v>58</v>
-      </c>
-      <c r="B66" s="6" t="s">
-        <v>140</v>
-      </c>
-      <c r="C66" s="6" t="s">
-        <v>134</v>
       </c>
       <c r="D66" s="8"/>
       <c r="E66" s="6" t="s">
-        <v>134</v>
-      </c>
-      <c r="F66" s="3"/>
+        <v>141</v>
+      </c>
+      <c r="F66" s="3" t="s">
+        <v>177</v>
+      </c>
       <c r="G66" s="4" t="s">
         <v>114</v>
       </c>
-      <c r="H66" s="18" t="s">
-        <v>114</v>
-      </c>
+      <c r="H66" s="21"/>
       <c r="I66" s="22">
-        <v>7.19</v>
+        <v>1</v>
       </c>
       <c r="J66" s="22">
-        <v>7.19</v>
+        <v>5</v>
       </c>
     </row>
     <row r="67" spans="1:10" s="2" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A67" s="14">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B67" s="6" t="s">
-        <v>190</v>
+        <v>140</v>
       </c>
       <c r="C67" s="6" t="s">
-        <v>191</v>
+        <v>134</v>
       </c>
       <c r="D67" s="8"/>
       <c r="E67" s="6" t="s">
-        <v>192</v>
+        <v>134</v>
       </c>
       <c r="F67" s="3"/>
       <c r="G67" s="4" t="s">
         <v>114</v>
       </c>
-      <c r="H67" s="18"/>
+      <c r="H67" s="18" t="s">
+        <v>114</v>
+      </c>
       <c r="I67" s="22">
+        <v>7.19</v>
+      </c>
+      <c r="J67" s="22">
+        <v>7.19</v>
+      </c>
+    </row>
+    <row r="68" spans="1:10" s="2" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A68" s="14">
+        <v>59</v>
+      </c>
+      <c r="B68" s="6" t="s">
+        <v>190</v>
+      </c>
+      <c r="C68" s="6" t="s">
+        <v>191</v>
+      </c>
+      <c r="D68" s="8"/>
+      <c r="E68" s="6" t="s">
+        <v>192</v>
+      </c>
+      <c r="F68" s="3"/>
+      <c r="G68" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="H68" s="18"/>
+      <c r="I68" s="22">
         <v>2.5</v>
       </c>
-      <c r="J67" s="22">
+      <c r="J68" s="22">
         <v>25</v>
       </c>
     </row>
-    <row r="68" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="G68" s="16" t="s">
+    <row r="69" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="G69" s="16" t="s">
         <v>193</v>
       </c>
-      <c r="H68" s="16"/>
-      <c r="I68" s="16">
-        <f>SUM(I5:I67)</f>
-        <v>114.40516666666667</v>
-      </c>
-      <c r="J68" s="16">
-        <f>SUM(J5:J67)</f>
-        <v>852.79933333000008</v>
+      <c r="H69" s="16"/>
+      <c r="I69" s="16">
+        <f>SUM(I5:I68)</f>
+        <v>114.50516666666668</v>
+      </c>
+      <c r="J69" s="16">
+        <f>SUM(J5:J68)</f>
+        <v>853.04933333000008</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="8">
     <mergeCell ref="I3:J3"/>
     <mergeCell ref="A1:J2"/>
-    <mergeCell ref="A43:H43"/>
-    <mergeCell ref="A53:H53"/>
+    <mergeCell ref="A44:H44"/>
+    <mergeCell ref="A54:H54"/>
     <mergeCell ref="A4:H4"/>
-    <mergeCell ref="A16:H16"/>
-    <mergeCell ref="A25:H25"/>
-    <mergeCell ref="A33:H33"/>
+    <mergeCell ref="A17:H17"/>
+    <mergeCell ref="A26:H26"/>
+    <mergeCell ref="A34:H34"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="G5" r:id="rId1" xr:uid="{318B6C4A-91DA-9E46-8E46-B8AEED1DCE8F}"/>
     <hyperlink ref="G7" r:id="rId2" xr:uid="{EC826376-44AD-8A44-A52C-3E440F3A7A2B}"/>
     <hyperlink ref="G8" r:id="rId3" xr:uid="{CE852A53-A9E0-EB4D-9B35-F1DD2D688ED7}"/>
-    <hyperlink ref="G10" r:id="rId4" xr:uid="{B9824164-545A-A447-B198-10945E963DAD}"/>
-    <hyperlink ref="G11" r:id="rId5" xr:uid="{B4D6765F-3917-FC40-90AE-7C3D6C1A6AC8}"/>
-    <hyperlink ref="G12" r:id="rId6" xr:uid="{EBB8A8BC-DFD2-3647-A406-A68875DAF9BD}"/>
-    <hyperlink ref="G13" r:id="rId7" xr:uid="{C2DD84EA-2DC6-1648-B0A9-45D29ABCD4B7}"/>
-    <hyperlink ref="G14" r:id="rId8" xr:uid="{3852C9A9-29DE-454F-9064-670966183131}"/>
-    <hyperlink ref="G15" r:id="rId9" xr:uid="{8E79DF2E-48DB-5343-8725-9EBC8479C3EE}"/>
-    <hyperlink ref="G17" r:id="rId10" xr:uid="{4097543D-3138-6B42-AB7C-A1133F869746}"/>
-    <hyperlink ref="G18" r:id="rId11" xr:uid="{32E17C97-C9D4-CC49-BAD2-C1EF7AF54FB5}"/>
-    <hyperlink ref="G19" r:id="rId12" xr:uid="{F79D8A94-C1CD-B54C-B7D7-125C6EA96AF4}"/>
-    <hyperlink ref="G20" r:id="rId13" xr:uid="{125A585B-58CB-B34D-9E97-B52879735699}"/>
-    <hyperlink ref="G21" r:id="rId14" xr:uid="{8C0DEBC4-ED4A-6849-A33E-E2AB3741CECF}"/>
-    <hyperlink ref="G22" r:id="rId15" xr:uid="{EED43844-CB6F-FE45-A828-338E6BE43422}"/>
-    <hyperlink ref="G23" r:id="rId16" xr:uid="{A67F3F64-177D-CB49-AD58-5F17E058A77A}"/>
-    <hyperlink ref="G49" r:id="rId17" xr:uid="{26106AE1-1FA7-E14A-838F-53E19B7CCE97}"/>
-    <hyperlink ref="G24" r:id="rId18" xr:uid="{59AA74E0-F75A-3C45-8B36-A539A51F8438}"/>
-    <hyperlink ref="G26" r:id="rId19" xr:uid="{54B3ACDF-1551-0F4E-A780-6DA35EB20361}"/>
-    <hyperlink ref="G27" r:id="rId20" xr:uid="{9D0D499A-6B3C-784C-9423-C21F14A7402F}"/>
-    <hyperlink ref="G28" r:id="rId21" xr:uid="{69E30EE6-91D1-0B40-AB9C-A0F37865C790}"/>
-    <hyperlink ref="G29" r:id="rId22" xr:uid="{C66A45AA-D0EA-534A-A813-22EAB56F5E83}"/>
-    <hyperlink ref="G30" r:id="rId23" xr:uid="{4F60F94A-490D-CA4F-B555-020CC8038A12}"/>
-    <hyperlink ref="G31" r:id="rId24" xr:uid="{92EA5DFD-5C62-C249-A4BA-C8D51F259335}"/>
-    <hyperlink ref="G32" r:id="rId25" xr:uid="{DAA65368-96A4-F649-80C6-47C27D6E77EB}"/>
-    <hyperlink ref="G34" r:id="rId26" xr:uid="{BCFBE50A-4F43-E041-A2B0-3A39ACB29628}"/>
-    <hyperlink ref="G36" r:id="rId27" xr:uid="{28B79E98-1696-BE46-87D2-E047D9390A4B}"/>
-    <hyperlink ref="G38" r:id="rId28" xr:uid="{060B0E4E-853A-4744-8793-0FB142CBAFA5}"/>
-    <hyperlink ref="G39" r:id="rId29" xr:uid="{704EA759-3F24-1E43-9225-F3EF4AF1D8AE}"/>
-    <hyperlink ref="G40" r:id="rId30" xr:uid="{51DEB24F-F2D8-034B-B4CE-B862AFD8AEF4}"/>
-    <hyperlink ref="G42" r:id="rId31" xr:uid="{2699EBE7-D782-624D-89C6-8E001041169F}"/>
-    <hyperlink ref="G44" r:id="rId32" xr:uid="{627C4F45-41F7-F540-B4E2-2728848CDE60}"/>
-    <hyperlink ref="G51" r:id="rId33" xr:uid="{4D237FA4-6FE9-5A4C-8713-4FCD965F5231}"/>
-    <hyperlink ref="G52" r:id="rId34" xr:uid="{4E031D5E-4B15-E646-AA8E-47A65B6EFF79}"/>
-    <hyperlink ref="G62" r:id="rId35" xr:uid="{FDE7FB9D-D7E4-7544-96B1-C85422C1CAA7}"/>
-    <hyperlink ref="G61" r:id="rId36" xr:uid="{6AE9298E-B5B2-DD44-8E1C-0E89BF893AE6}"/>
-    <hyperlink ref="G59" r:id="rId37" xr:uid="{7F05D5E5-E6BA-CD40-BF00-3E6A222ACF58}"/>
-    <hyperlink ref="G55" r:id="rId38" xr:uid="{81004994-FC78-8547-9153-583C44AE1D76}"/>
-    <hyperlink ref="G58" r:id="rId39" xr:uid="{A7A3D3E7-DB98-9846-9837-4F92A5AEC05B}"/>
-    <hyperlink ref="G63" r:id="rId40" xr:uid="{A4C11252-F340-8C41-94EA-7F54CBE97C72}"/>
-    <hyperlink ref="G64" r:id="rId41" xr:uid="{9754C7AB-196A-6549-BEAD-D36381163F48}"/>
-    <hyperlink ref="G67" r:id="rId42" xr:uid="{4398D883-8521-194B-8F9B-83CB9FAC708C}"/>
-    <hyperlink ref="G60" r:id="rId43" xr:uid="{8121FC13-B5AD-DE45-B596-7A654553B8E1}"/>
-    <hyperlink ref="G56" r:id="rId44" xr:uid="{5239B69E-6ECC-9A44-AB79-B03D6976AB4B}"/>
-    <hyperlink ref="G65" r:id="rId45" xr:uid="{2649F7DB-4C28-0842-86F0-046A8CBD0D7F}"/>
-    <hyperlink ref="G57" r:id="rId46" xr:uid="{8E7EBB42-4FF3-2040-B177-E71E2A9B513B}"/>
-    <hyperlink ref="G9" r:id="rId47" xr:uid="{4D3355E8-5A36-174A-A71D-DB31B3BDB127}"/>
-    <hyperlink ref="G37" r:id="rId48" xr:uid="{565D2868-B2F4-4147-8B2C-9DA2839B402A}"/>
+    <hyperlink ref="G11" r:id="rId4" xr:uid="{B9824164-545A-A447-B198-10945E963DAD}"/>
+    <hyperlink ref="G12" r:id="rId5" xr:uid="{B4D6765F-3917-FC40-90AE-7C3D6C1A6AC8}"/>
+    <hyperlink ref="G13" r:id="rId6" xr:uid="{EBB8A8BC-DFD2-3647-A406-A68875DAF9BD}"/>
+    <hyperlink ref="G14" r:id="rId7" xr:uid="{C2DD84EA-2DC6-1648-B0A9-45D29ABCD4B7}"/>
+    <hyperlink ref="G15" r:id="rId8" xr:uid="{3852C9A9-29DE-454F-9064-670966183131}"/>
+    <hyperlink ref="G16" r:id="rId9" xr:uid="{8E79DF2E-48DB-5343-8725-9EBC8479C3EE}"/>
+    <hyperlink ref="G18" r:id="rId10" xr:uid="{4097543D-3138-6B42-AB7C-A1133F869746}"/>
+    <hyperlink ref="G19" r:id="rId11" xr:uid="{32E17C97-C9D4-CC49-BAD2-C1EF7AF54FB5}"/>
+    <hyperlink ref="G20" r:id="rId12" xr:uid="{F79D8A94-C1CD-B54C-B7D7-125C6EA96AF4}"/>
+    <hyperlink ref="G21" r:id="rId13" xr:uid="{125A585B-58CB-B34D-9E97-B52879735699}"/>
+    <hyperlink ref="G22" r:id="rId14" xr:uid="{8C0DEBC4-ED4A-6849-A33E-E2AB3741CECF}"/>
+    <hyperlink ref="G23" r:id="rId15" xr:uid="{EED43844-CB6F-FE45-A828-338E6BE43422}"/>
+    <hyperlink ref="G24" r:id="rId16" xr:uid="{A67F3F64-177D-CB49-AD58-5F17E058A77A}"/>
+    <hyperlink ref="G50" r:id="rId17" xr:uid="{26106AE1-1FA7-E14A-838F-53E19B7CCE97}"/>
+    <hyperlink ref="G25" r:id="rId18" xr:uid="{59AA74E0-F75A-3C45-8B36-A539A51F8438}"/>
+    <hyperlink ref="G27" r:id="rId19" xr:uid="{54B3ACDF-1551-0F4E-A780-6DA35EB20361}"/>
+    <hyperlink ref="G28" r:id="rId20" xr:uid="{9D0D499A-6B3C-784C-9423-C21F14A7402F}"/>
+    <hyperlink ref="G29" r:id="rId21" xr:uid="{69E30EE6-91D1-0B40-AB9C-A0F37865C790}"/>
+    <hyperlink ref="G30" r:id="rId22" xr:uid="{C66A45AA-D0EA-534A-A813-22EAB56F5E83}"/>
+    <hyperlink ref="G31" r:id="rId23" xr:uid="{4F60F94A-490D-CA4F-B555-020CC8038A12}"/>
+    <hyperlink ref="G32" r:id="rId24" xr:uid="{92EA5DFD-5C62-C249-A4BA-C8D51F259335}"/>
+    <hyperlink ref="G33" r:id="rId25" xr:uid="{DAA65368-96A4-F649-80C6-47C27D6E77EB}"/>
+    <hyperlink ref="G35" r:id="rId26" xr:uid="{BCFBE50A-4F43-E041-A2B0-3A39ACB29628}"/>
+    <hyperlink ref="G37" r:id="rId27" xr:uid="{28B79E98-1696-BE46-87D2-E047D9390A4B}"/>
+    <hyperlink ref="G39" r:id="rId28" xr:uid="{060B0E4E-853A-4744-8793-0FB142CBAFA5}"/>
+    <hyperlink ref="G40" r:id="rId29" xr:uid="{704EA759-3F24-1E43-9225-F3EF4AF1D8AE}"/>
+    <hyperlink ref="G41" r:id="rId30" xr:uid="{51DEB24F-F2D8-034B-B4CE-B862AFD8AEF4}"/>
+    <hyperlink ref="G43" r:id="rId31" xr:uid="{2699EBE7-D782-624D-89C6-8E001041169F}"/>
+    <hyperlink ref="G45" r:id="rId32" xr:uid="{627C4F45-41F7-F540-B4E2-2728848CDE60}"/>
+    <hyperlink ref="G52" r:id="rId33" xr:uid="{4D237FA4-6FE9-5A4C-8713-4FCD965F5231}"/>
+    <hyperlink ref="G53" r:id="rId34" xr:uid="{4E031D5E-4B15-E646-AA8E-47A65B6EFF79}"/>
+    <hyperlink ref="G63" r:id="rId35" xr:uid="{FDE7FB9D-D7E4-7544-96B1-C85422C1CAA7}"/>
+    <hyperlink ref="G62" r:id="rId36" xr:uid="{6AE9298E-B5B2-DD44-8E1C-0E89BF893AE6}"/>
+    <hyperlink ref="G60" r:id="rId37" xr:uid="{7F05D5E5-E6BA-CD40-BF00-3E6A222ACF58}"/>
+    <hyperlink ref="G56" r:id="rId38" xr:uid="{81004994-FC78-8547-9153-583C44AE1D76}"/>
+    <hyperlink ref="G59" r:id="rId39" xr:uid="{A7A3D3E7-DB98-9846-9837-4F92A5AEC05B}"/>
+    <hyperlink ref="G64" r:id="rId40" xr:uid="{A4C11252-F340-8C41-94EA-7F54CBE97C72}"/>
+    <hyperlink ref="G65" r:id="rId41" xr:uid="{9754C7AB-196A-6549-BEAD-D36381163F48}"/>
+    <hyperlink ref="G68" r:id="rId42" xr:uid="{4398D883-8521-194B-8F9B-83CB9FAC708C}"/>
+    <hyperlink ref="G61" r:id="rId43" xr:uid="{8121FC13-B5AD-DE45-B596-7A654553B8E1}"/>
+    <hyperlink ref="G57" r:id="rId44" xr:uid="{5239B69E-6ECC-9A44-AB79-B03D6976AB4B}"/>
+    <hyperlink ref="G66" r:id="rId45" xr:uid="{2649F7DB-4C28-0842-86F0-046A8CBD0D7F}"/>
+    <hyperlink ref="G58" r:id="rId46" xr:uid="{8E7EBB42-4FF3-2040-B177-E71E2A9B513B}"/>
+    <hyperlink ref="G10" r:id="rId47" xr:uid="{4D3355E8-5A36-174A-A71D-DB31B3BDB127}"/>
+    <hyperlink ref="G38" r:id="rId48" xr:uid="{565D2868-B2F4-4147-8B2C-9DA2839B402A}"/>
     <hyperlink ref="G6" r:id="rId49" xr:uid="{41337B6D-A726-404F-8E3A-A7297AAEF553}"/>
-    <hyperlink ref="G45" r:id="rId50" xr:uid="{34D85EC0-0AEE-374A-B6A1-76DF8A07B165}"/>
-    <hyperlink ref="G46" r:id="rId51" xr:uid="{EDB9A295-1581-C24A-88A3-E0CC212C0DDD}"/>
-    <hyperlink ref="G47" r:id="rId52" xr:uid="{6DE2C368-613C-9D4D-9F84-6D0DBC951923}"/>
-    <hyperlink ref="G48" r:id="rId53" xr:uid="{4DC302ED-59A9-2449-A361-F29906F9C3AE}"/>
-    <hyperlink ref="H32" r:id="rId54" xr:uid="{D70B5C5F-26F0-0B41-8C17-1CC14ADA3FE6}"/>
-    <hyperlink ref="H34" r:id="rId55" xr:uid="{0641F1EB-124F-B04D-A94A-758F384DED86}"/>
-    <hyperlink ref="H35" r:id="rId56" xr:uid="{DB0D0FF9-650C-9047-8B87-64100B2B793F}"/>
-    <hyperlink ref="H36" r:id="rId57" xr:uid="{C2D15776-74B0-F248-A49B-2B60EC4E9F50}"/>
-    <hyperlink ref="H37" r:id="rId58" xr:uid="{7FCBF6EC-A974-3C4D-8ECC-BADD5D52FD8F}"/>
-    <hyperlink ref="H41" r:id="rId59" xr:uid="{FF2327CA-6C12-1B4D-9F3D-A6892FDF93AA}"/>
-    <hyperlink ref="G41" r:id="rId60" xr:uid="{A3991D56-3C5A-D24F-9BF4-72B691163E2E}"/>
-    <hyperlink ref="H42" r:id="rId61" xr:uid="{85C3CCAE-AE34-6F4D-BB81-D0542993FD86}"/>
-    <hyperlink ref="G50" r:id="rId62" xr:uid="{6D279AE6-1632-D949-AF1B-D9B01BEE22D5}"/>
-    <hyperlink ref="G54" r:id="rId63" xr:uid="{77ED00C2-AEB9-AF46-BAD4-47C057542ED7}"/>
-    <hyperlink ref="H60" r:id="rId64" xr:uid="{7E92FC71-1828-1347-8A0C-006F6C8E33D9}"/>
-    <hyperlink ref="H62" r:id="rId65" xr:uid="{765DA2F2-534C-F04A-83EE-6DE4C93A616F}"/>
-    <hyperlink ref="H63" r:id="rId66" xr:uid="{2FF58D32-1303-3741-8980-398B83460ED3}"/>
-    <hyperlink ref="H64" r:id="rId67" xr:uid="{26EDE05F-D1A0-2C4A-8936-BE0E610D5348}"/>
-    <hyperlink ref="G66" r:id="rId68" xr:uid="{1F44837E-6CDE-1F4D-ADC9-348EB68867C4}"/>
-    <hyperlink ref="H66" r:id="rId69" xr:uid="{A9E4EEEA-BAD5-8044-925B-73291B6B46E9}"/>
+    <hyperlink ref="G46" r:id="rId50" xr:uid="{34D85EC0-0AEE-374A-B6A1-76DF8A07B165}"/>
+    <hyperlink ref="G47" r:id="rId51" xr:uid="{EDB9A295-1581-C24A-88A3-E0CC212C0DDD}"/>
+    <hyperlink ref="G48" r:id="rId52" xr:uid="{6DE2C368-613C-9D4D-9F84-6D0DBC951923}"/>
+    <hyperlink ref="G49" r:id="rId53" xr:uid="{4DC302ED-59A9-2449-A361-F29906F9C3AE}"/>
+    <hyperlink ref="H33" r:id="rId54" xr:uid="{D70B5C5F-26F0-0B41-8C17-1CC14ADA3FE6}"/>
+    <hyperlink ref="H35" r:id="rId55" xr:uid="{0641F1EB-124F-B04D-A94A-758F384DED86}"/>
+    <hyperlink ref="H36" r:id="rId56" xr:uid="{DB0D0FF9-650C-9047-8B87-64100B2B793F}"/>
+    <hyperlink ref="H37" r:id="rId57" xr:uid="{C2D15776-74B0-F248-A49B-2B60EC4E9F50}"/>
+    <hyperlink ref="H38" r:id="rId58" xr:uid="{7FCBF6EC-A974-3C4D-8ECC-BADD5D52FD8F}"/>
+    <hyperlink ref="H42" r:id="rId59" xr:uid="{FF2327CA-6C12-1B4D-9F3D-A6892FDF93AA}"/>
+    <hyperlink ref="G42" r:id="rId60" xr:uid="{A3991D56-3C5A-D24F-9BF4-72B691163E2E}"/>
+    <hyperlink ref="H43" r:id="rId61" xr:uid="{85C3CCAE-AE34-6F4D-BB81-D0542993FD86}"/>
+    <hyperlink ref="G51" r:id="rId62" xr:uid="{6D279AE6-1632-D949-AF1B-D9B01BEE22D5}"/>
+    <hyperlink ref="G55" r:id="rId63" xr:uid="{77ED00C2-AEB9-AF46-BAD4-47C057542ED7}"/>
+    <hyperlink ref="H61" r:id="rId64" xr:uid="{7E92FC71-1828-1347-8A0C-006F6C8E33D9}"/>
+    <hyperlink ref="H63" r:id="rId65" xr:uid="{765DA2F2-534C-F04A-83EE-6DE4C93A616F}"/>
+    <hyperlink ref="H64" r:id="rId66" xr:uid="{2FF58D32-1303-3741-8980-398B83460ED3}"/>
+    <hyperlink ref="H65" r:id="rId67" xr:uid="{26EDE05F-D1A0-2C4A-8936-BE0E610D5348}"/>
+    <hyperlink ref="G67" r:id="rId68" xr:uid="{1F44837E-6CDE-1F4D-ADC9-348EB68867C4}"/>
+    <hyperlink ref="H67" r:id="rId69" xr:uid="{A9E4EEEA-BAD5-8044-925B-73291B6B46E9}"/>
+    <hyperlink ref="G9" r:id="rId70" xr:uid="{B0E09EC5-69E6-604E-8798-614507E33CDD}"/>
   </hyperlinks>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
   <pageSetup scale="40" fitToHeight="4" orientation="portrait" copies="2"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>
-  <drawing r:id="rId70"/>
+  <drawing r:id="rId71"/>
 </worksheet>
 </file>
</xml_diff>